<commit_message>
Done MVC basic layout
</commit_message>
<xml_diff>
--- a/Documentation/Sprint Documentation.xlsx
+++ b/Documentation/Sprint Documentation.xlsx
@@ -1,13 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\0950141\I221\Groupproj\Documentation\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{534F9732-C56F-45F7-AED4-0F8A154671A1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Burndown Chart" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="Product Backlog" sheetId="2" r:id="rId5"/>
+    <sheet name="Burndown Chart" sheetId="1" r:id="rId1"/>
+    <sheet name="Product Backlog" sheetId="2" r:id="rId2"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId6" roundtripDataSignature="AMtx7mjTACquWQvIaZTSYFILUJIUo8aUqQ=="/>
@@ -249,50 +258,59 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="11">
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="11"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="Arial"/>
     </font>
-    <font/>
     <font>
+      <sz val="11"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
     <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
+      <sz val="11"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF24292F"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="9.0"/>
+      <sz val="9"/>
       <color rgb="FF24292F"/>
       <name val="Ui-monospace"/>
     </font>
@@ -302,7 +320,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -312,7 +330,13 @@
     </fill>
   </fills>
   <borders count="16">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
@@ -326,16 +350,21 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
@@ -345,6 +374,7 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -353,37 +383,58 @@
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
+      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -392,41 +443,55 @@
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
+      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
+      <right/>
+      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
+      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
+      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -438,200 +503,184 @@
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
+      <bottom/>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="3" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="5" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="6" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="6" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="7" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="8" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="9" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="10" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="11" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="12" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="12" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="13" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="5" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="6" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="11" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="12" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="14" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="2" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="2" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="2" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="3" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="5" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="6" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="15" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="15" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+  <cellXfs count="75">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="9" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="8" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="4" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="9" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="11" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="12" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="10" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="10" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="15" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="5" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="5" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="14" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="2" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="9" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="15" fillId="2" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="12" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="12" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="12" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="13" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" shrinkToFit="0" vertical="top" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="top"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" shrinkToFit="0" vertical="top" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="top"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="1"/>
+  <c:style val="2"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -640,7 +689,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr lvl="0">
-              <a:defRPr b="0" i="0" sz="1400">
+              <a:defRPr sz="1400" b="0" i="0">
                 <a:solidFill>
                   <a:srgbClr val="757575"/>
                 </a:solidFill>
@@ -648,7 +697,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr b="0" i="0" sz="1400">
+              <a:rPr lang="en-NZ" sz="1400" b="0" i="0">
                 <a:solidFill>
                   <a:srgbClr val="757575"/>
                 </a:solidFill>
@@ -663,15 +712,18 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.4094930008748907"/>
-          <c:y val="0.0"/>
+          <c:x val="0.40949300087489071"/>
+          <c:y val="0"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="1"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -679,7 +731,7 @@
             <c:v>Actual Remaining Effort</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln cmpd="sng" w="28575">
+            <a:ln w="28575" cmpd="sng">
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
@@ -691,10 +743,45 @@
           <c:val>
             <c:numRef>
               <c:f>'Burndown Chart'!$C$19:$K$19</c:f>
-              <c:numCache/>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>15</c:v>
+                </c:pt>
+              </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-2EC4-47A5-ABED-C90CB64A911B}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -703,7 +790,7 @@
             <c:v>Estimated Remaining Effort</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln cmpd="sng" w="28575">
+            <a:ln w="28575" cmpd="sng">
               <a:solidFill>
                 <a:schemeClr val="accent2"/>
               </a:solidFill>
@@ -715,11 +802,55 @@
           <c:val>
             <c:numRef>
               <c:f>'Burndown Chart'!$C$20:$K$20</c:f>
-              <c:numCache/>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>23.625</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20.25</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16.875</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>13.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10.125</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.75</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.375</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-2EC4-47A5-ABED-C90CB64A911B}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
         <c:axId val="2138243776"/>
         <c:axId val="1908582515"/>
       </c:lineChart>
@@ -737,7 +868,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr lvl="0">
-                  <a:defRPr b="0" i="0" sz="1000">
+                  <a:defRPr sz="1000" b="0" i="0">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
@@ -745,7 +876,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr b="0" i="0" sz="1000">
+                  <a:rPr lang="en-NZ" sz="1000" b="0" i="0">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
@@ -761,22 +892,28 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
-        <c:spPr/>
+        <c:tickLblPos val="nextTo"/>
         <c:txPr>
           <a:bodyPr/>
           <a:lstStyle/>
           <a:p>
             <a:pPr lvl="0">
-              <a:defRPr b="0" i="0" sz="900">
+              <a:defRPr sz="900" b="0" i="0">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
               </a:defRPr>
             </a:pPr>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1908582515"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
         <c:axId val="1908582515"/>
@@ -801,7 +938,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr lvl="0">
-                  <a:defRPr b="0" i="0" sz="1000">
+                  <a:defRPr sz="1000" b="0" i="0">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
@@ -809,7 +946,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr b="0" i="0" sz="1000">
+                  <a:rPr lang="en-NZ" sz="1000" b="0" i="0">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
@@ -834,16 +971,19 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr lvl="0">
-              <a:defRPr b="0" i="0" sz="900">
+              <a:defRPr sz="900" b="0" i="0">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
               </a:defRPr>
             </a:pPr>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="2138243776"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -854,23 +994,31 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr lvl="0">
-            <a:defRPr b="0" i="0" sz="900">
+            <a:defRPr sz="900" b="0" i="0">
               <a:solidFill>
                 <a:srgbClr val="1A1A1A"/>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
             </a:defRPr>
           </a:pPr>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="1"/>
   </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>13</xdr:col>
@@ -879,9 +1027,15 @@
       <xdr:rowOff>542925</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="4371975" cy="2838450"/>
-    <xdr:graphicFrame>
+    <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="1278677386" name="Chart 1" title="Chart"/>
+        <xdr:cNvPr id="1278677386" name="Chart 1" title="Chart">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00008A11374C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -890,7 +1044,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart r:id="rId1"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -899,12 +1053,8 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -1094,46 +1244,48 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B1:L1007"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:F18"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="4.63"/>
-    <col customWidth="1" min="2" max="2" width="29.75"/>
-    <col customWidth="1" min="3" max="3" width="9.13"/>
-    <col customWidth="1" min="4" max="4" width="6.63"/>
-    <col customWidth="1" min="5" max="5" width="6.5"/>
-    <col customWidth="1" min="6" max="6" width="6.38"/>
-    <col customWidth="1" min="7" max="7" width="6.5"/>
-    <col customWidth="1" min="8" max="8" width="6.75"/>
-    <col customWidth="1" min="9" max="9" width="6.63"/>
-    <col customWidth="1" min="10" max="11" width="6.75"/>
-    <col customWidth="1" min="12" max="12" width="6.5"/>
-    <col customWidth="1" min="13" max="13" width="5.63"/>
-    <col customWidth="1" min="14" max="14" width="6.0"/>
-    <col customWidth="1" min="15" max="15" width="5.38"/>
-    <col customWidth="1" min="16" max="16" width="5.75"/>
-    <col customWidth="1" min="17" max="17" width="5.0"/>
-    <col customWidth="1" min="18" max="18" width="5.38"/>
-    <col customWidth="1" min="19" max="19" width="4.5"/>
-    <col customWidth="1" min="20" max="20" width="4.75"/>
-    <col customWidth="1" min="21" max="21" width="5.63"/>
-    <col customWidth="1" min="22" max="22" width="5.13"/>
-    <col customWidth="1" min="23" max="24" width="5.25"/>
-    <col customWidth="1" min="25" max="25" width="5.0"/>
-    <col customWidth="1" min="26" max="26" width="5.25"/>
+    <col min="1" max="1" width="4.625" customWidth="1"/>
+    <col min="2" max="2" width="29.75" customWidth="1"/>
+    <col min="3" max="3" width="9.125" customWidth="1"/>
+    <col min="4" max="4" width="6.625" customWidth="1"/>
+    <col min="5" max="5" width="6.5" customWidth="1"/>
+    <col min="6" max="6" width="6.375" customWidth="1"/>
+    <col min="7" max="7" width="6.5" customWidth="1"/>
+    <col min="8" max="8" width="6.75" customWidth="1"/>
+    <col min="9" max="9" width="6.625" customWidth="1"/>
+    <col min="10" max="11" width="6.75" customWidth="1"/>
+    <col min="12" max="12" width="6.5" customWidth="1"/>
+    <col min="13" max="13" width="5.625" customWidth="1"/>
+    <col min="14" max="14" width="6" customWidth="1"/>
+    <col min="15" max="15" width="5.375" customWidth="1"/>
+    <col min="16" max="16" width="5.75" customWidth="1"/>
+    <col min="17" max="17" width="5" customWidth="1"/>
+    <col min="18" max="18" width="5.375" customWidth="1"/>
+    <col min="19" max="19" width="4.5" customWidth="1"/>
+    <col min="20" max="20" width="4.75" customWidth="1"/>
+    <col min="21" max="21" width="5.625" customWidth="1"/>
+    <col min="22" max="22" width="5.125" customWidth="1"/>
+    <col min="23" max="24" width="5.25" customWidth="1"/>
+    <col min="25" max="25" width="5" customWidth="1"/>
+    <col min="26" max="26" width="5.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="59.25" customHeight="1">
+    <row r="1" spans="2:12" ht="59.25" customHeight="1">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1168,325 +1320,374 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" ht="21.75" customHeight="1">
+    <row r="2" spans="2:12" ht="21.75" customHeight="1">
       <c r="B2" s="5" t="s">
         <v>11</v>
       </c>
       <c r="C2" s="6">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="D2" s="7">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E2" s="7">
-        <v>3.0</v>
-      </c>
-      <c r="F2" s="8"/>
+        <v>3</v>
+      </c>
+      <c r="F2" s="7">
+        <v>3</v>
+      </c>
       <c r="G2" s="8"/>
       <c r="H2" s="8"/>
       <c r="I2" s="8"/>
       <c r="J2" s="8"/>
       <c r="K2" s="8"/>
       <c r="L2" s="9">
-        <f t="shared" ref="L2:L18" si="1">SUM(D2:K2)</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" ht="18.75" customHeight="1">
+        <f t="shared" ref="L2:L18" si="0">SUM(D2:K2)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="2:12" ht="18.75" customHeight="1">
       <c r="B3" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C3" s="10">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="D3" s="11">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E3" s="11">
-        <v>1.0</v>
+        <v>1</v>
+      </c>
+      <c r="F3" s="11">
+        <v>1</v>
       </c>
       <c r="L3" s="12">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" ht="20.25" customHeight="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12" ht="20.25" customHeight="1">
       <c r="B4" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C4" s="10">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="D4" s="11">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E4" s="11">
-        <v>1.0</v>
+        <v>1</v>
+      </c>
+      <c r="F4" s="11">
+        <v>1</v>
       </c>
       <c r="L4" s="12">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" ht="20.25" customHeight="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" ht="20.25" customHeight="1">
       <c r="B5" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C5" s="10">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="D5" s="11">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E5" s="13">
-        <v>0.0</v>
+        <v>0</v>
+      </c>
+      <c r="F5" s="13">
+        <v>0</v>
       </c>
       <c r="L5" s="12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" ht="18.75" customHeight="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" ht="18.75" customHeight="1">
       <c r="B6" s="5" t="s">
         <v>15</v>
       </c>
       <c r="C6" s="10">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="D6" s="11">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E6" s="13">
         <v>0.25</v>
       </c>
+      <c r="F6" s="13">
+        <v>0.25</v>
+      </c>
       <c r="L6" s="12">
-        <f t="shared" si="1"/>
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="7" ht="20.25" customHeight="1">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" ht="20.25" customHeight="1">
       <c r="B7" s="5" t="s">
         <v>16</v>
       </c>
       <c r="C7" s="10">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="D7" s="11">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E7" s="13">
         <v>0.25</v>
       </c>
+      <c r="F7" s="13">
+        <v>0.25</v>
+      </c>
       <c r="L7" s="12">
-        <f t="shared" si="1"/>
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="8" ht="19.5" customHeight="1">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12" ht="19.5" customHeight="1">
       <c r="B8" s="5" t="s">
         <v>17</v>
       </c>
       <c r="C8" s="10">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="D8" s="11">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E8" s="11">
-        <v>0.0</v>
+        <v>0</v>
+      </c>
+      <c r="F8" s="11">
+        <v>0</v>
       </c>
       <c r="L8" s="12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" ht="18.0" customHeight="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" ht="18" customHeight="1">
       <c r="B9" s="5" t="s">
         <v>18</v>
       </c>
       <c r="C9" s="10">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="D9" s="11">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E9" s="13">
         <v>0.5</v>
       </c>
+      <c r="F9" s="13">
+        <v>0.5</v>
+      </c>
       <c r="L9" s="12">
-        <f t="shared" si="1"/>
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="10" ht="19.5" customHeight="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12" ht="19.5" customHeight="1">
       <c r="B10" s="14" t="s">
         <v>19</v>
       </c>
       <c r="C10" s="10">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="D10" s="11">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E10" s="11">
-        <v>0.0</v>
+        <v>0</v>
+      </c>
+      <c r="F10" s="11">
+        <v>0</v>
       </c>
       <c r="L10" s="12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" ht="21.75" customHeight="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12" ht="21.75" customHeight="1">
       <c r="B11" s="5" t="s">
         <v>20</v>
       </c>
       <c r="C11" s="10">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="D11" s="11">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E11" s="11">
-        <v>0.0</v>
+        <v>0</v>
+      </c>
+      <c r="F11" s="11">
+        <v>0</v>
       </c>
       <c r="L11" s="12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" ht="19.5" customHeight="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" ht="19.5" customHeight="1">
       <c r="B12" s="15" t="s">
         <v>21</v>
       </c>
       <c r="C12" s="10">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="D12" s="11">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E12" s="11">
-        <v>0.0</v>
+        <v>0</v>
+      </c>
+      <c r="F12" s="11">
+        <v>0</v>
       </c>
       <c r="L12" s="12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" ht="18.0" customHeight="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12" ht="18" customHeight="1">
       <c r="B13" s="15" t="s">
         <v>22</v>
       </c>
       <c r="C13" s="10">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="D13" s="11">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E13" s="11">
-        <v>0.0</v>
+        <v>0</v>
+      </c>
+      <c r="F13" s="11">
+        <v>0</v>
       </c>
       <c r="L13" s="12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" ht="28.5" customHeight="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="2:12" ht="28.5" customHeight="1">
       <c r="B14" s="15" t="s">
         <v>23</v>
       </c>
       <c r="C14" s="10">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="D14" s="11">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E14" s="11">
-        <v>0.0</v>
+        <v>0</v>
+      </c>
+      <c r="F14" s="11">
+        <v>0</v>
       </c>
       <c r="L14" s="12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" ht="28.5" customHeight="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12" ht="28.5" customHeight="1">
       <c r="B15" s="15" t="s">
         <v>24</v>
       </c>
       <c r="C15" s="10">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="D15" s="11">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E15" s="11">
-        <v>0.0</v>
+        <v>0</v>
+      </c>
+      <c r="F15" s="11">
+        <v>0</v>
       </c>
       <c r="L15" s="12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" ht="31.5" customHeight="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="2:12" ht="31.5" customHeight="1">
       <c r="B16" s="15" t="s">
         <v>25</v>
       </c>
       <c r="C16" s="10">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="D16" s="11">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E16" s="11">
-        <v>0.0</v>
+        <v>0</v>
+      </c>
+      <c r="F16" s="11">
+        <v>0</v>
       </c>
       <c r="L16" s="12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" ht="28.5" customHeight="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:12" ht="28.5" customHeight="1">
       <c r="B17" s="15" t="s">
         <v>26</v>
       </c>
       <c r="C17" s="10">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="D17" s="11">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E17" s="11">
-        <v>0.0</v>
+        <v>0</v>
+      </c>
+      <c r="F17" s="11">
+        <v>0</v>
       </c>
       <c r="L17" s="12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" ht="28.5" customHeight="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:12" ht="28.5" customHeight="1">
       <c r="B18" s="16" t="s">
         <v>27</v>
       </c>
       <c r="C18" s="17">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="D18" s="18">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E18" s="18">
-        <v>0.0</v>
-      </c>
-      <c r="F18" s="19"/>
+        <v>0</v>
+      </c>
+      <c r="F18" s="18">
+        <v>0</v>
+      </c>
       <c r="G18" s="19"/>
       <c r="H18" s="19"/>
       <c r="I18" s="19"/>
       <c r="J18" s="19"/>
       <c r="K18" s="19"/>
       <c r="L18" s="20">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" ht="22.5" customHeight="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="2:12" ht="22.5" customHeight="1">
       <c r="B19" s="21" t="s">
         <v>28</v>
       </c>
@@ -1495,39 +1696,39 @@
         <v>27</v>
       </c>
       <c r="D19" s="22">
-        <f t="shared" ref="D19:K19" si="2">C19-SUM(D2:D11)</f>
+        <f t="shared" ref="D19:K19" si="1">C19-SUM(D2:D11)</f>
         <v>27</v>
       </c>
       <c r="E19" s="22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>21</v>
       </c>
       <c r="F19" s="22">
-        <f t="shared" si="2"/>
-        <v>21</v>
+        <f t="shared" si="1"/>
+        <v>15</v>
       </c>
       <c r="G19" s="22">
-        <f t="shared" si="2"/>
-        <v>21</v>
+        <f t="shared" si="1"/>
+        <v>15</v>
       </c>
       <c r="H19" s="22">
-        <f t="shared" si="2"/>
-        <v>21</v>
+        <f t="shared" si="1"/>
+        <v>15</v>
       </c>
       <c r="I19" s="22">
-        <f t="shared" si="2"/>
-        <v>21</v>
+        <f t="shared" si="1"/>
+        <v>15</v>
       </c>
       <c r="J19" s="22">
-        <f t="shared" si="2"/>
-        <v>21</v>
+        <f t="shared" si="1"/>
+        <v>15</v>
       </c>
       <c r="K19" s="9">
-        <f t="shared" si="2"/>
-        <v>21</v>
-      </c>
-    </row>
-    <row r="20" ht="20.25" customHeight="1">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="2:12" ht="20.25" customHeight="1">
       <c r="B20" s="23" t="s">
         <v>29</v>
       </c>
@@ -1536,43 +1737,43 @@
         <v>27</v>
       </c>
       <c r="D20" s="24">
-        <f t="shared" ref="D20:K20" si="3">C20-($C$19/8)</f>
+        <f t="shared" ref="D20:K20" si="2">C20-($C$19/8)</f>
         <v>23.625</v>
       </c>
       <c r="E20" s="24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>20.25</v>
       </c>
       <c r="F20" s="24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>16.875</v>
       </c>
       <c r="G20" s="24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>13.5</v>
       </c>
       <c r="H20" s="24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>10.125</v>
       </c>
       <c r="I20" s="24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>6.75</v>
       </c>
       <c r="J20" s="24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>3.375</v>
       </c>
       <c r="K20" s="20">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" ht="15.75" customHeight="1"/>
-    <row r="29" ht="15.75" customHeight="1"/>
-    <row r="30" ht="15.75" customHeight="1"/>
-    <row r="31" ht="15.75" customHeight="1"/>
-    <row r="32" ht="15.75" customHeight="1"/>
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="2:12" ht="15.75" customHeight="1"/>
+    <row r="29" spans="2:12" ht="15.75" customHeight="1"/>
+    <row r="30" spans="2:12" ht="15.75" customHeight="1"/>
+    <row r="31" spans="2:12" ht="15.75" customHeight="1"/>
+    <row r="32" spans="2:12" ht="15.75" customHeight="1"/>
     <row r="33" ht="15.75" customHeight="1"/>
     <row r="34" ht="15.75" customHeight="1"/>
     <row r="35" ht="15.75" customHeight="1"/>
@@ -2549,631 +2750,638 @@
     <row r="1006" ht="15.75" customHeight="1"/>
     <row r="1007" ht="15.75" customHeight="1"/>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:L79"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="34.0"/>
-    <col customWidth="1" min="2" max="2" width="14.63"/>
-    <col customWidth="1" min="3" max="3" width="14.0"/>
+    <col min="1" max="1" width="34" customWidth="1"/>
+    <col min="2" max="2" width="14.625" customWidth="1"/>
+    <col min="3" max="3" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="36.0" customHeight="1">
+    <row r="1" spans="1:12" ht="36" customHeight="1">
       <c r="A1" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="74" t="s">
         <v>31</v>
       </c>
-      <c r="C1" s="27"/>
-      <c r="D1" s="28" t="s">
+      <c r="C1" s="57"/>
+      <c r="D1" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="E1" s="28" t="s">
+      <c r="E1" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="F1" s="29" t="s">
+      <c r="F1" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="G1" s="29" t="s">
+      <c r="G1" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="H1" s="29" t="s">
+      <c r="H1" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="I1" s="29" t="s">
+      <c r="I1" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="J1" s="29" t="s">
+      <c r="J1" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="K1" s="29" t="s">
+      <c r="K1" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="L1" s="30" t="s">
+      <c r="L1" s="28" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="2" ht="18.75" customHeight="1">
-      <c r="A2" s="31" t="s">
+    <row r="2" spans="1:12" ht="18.75" customHeight="1">
+      <c r="A2" s="69" t="s">
         <v>41</v>
       </c>
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="50" t="s">
         <v>42</v>
       </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="33">
-        <v>7.0</v>
-      </c>
-      <c r="E2" s="34">
-        <v>15.0</v>
-      </c>
-      <c r="F2" s="35">
-        <v>1.0</v>
-      </c>
-      <c r="G2" s="36">
-        <v>1.0</v>
-      </c>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
-      <c r="K2" s="37"/>
-      <c r="L2" s="38"/>
-    </row>
-    <row r="3" ht="19.5" customHeight="1">
-      <c r="A3" s="39"/>
-      <c r="B3" s="11" t="s">
+      <c r="C2" s="51"/>
+      <c r="D2" s="29">
+        <v>7</v>
+      </c>
+      <c r="E2" s="59">
+        <v>15</v>
+      </c>
+      <c r="F2" s="58">
+        <v>1</v>
+      </c>
+      <c r="G2" s="65">
+        <v>1</v>
+      </c>
+      <c r="H2" s="66"/>
+      <c r="I2" s="66"/>
+      <c r="J2" s="66"/>
+      <c r="K2" s="66"/>
+      <c r="L2" s="67"/>
+    </row>
+    <row r="3" spans="1:12" ht="19.5" customHeight="1">
+      <c r="A3" s="70"/>
+      <c r="B3" s="52" t="s">
         <v>43</v>
       </c>
-      <c r="D3" s="40">
-        <v>2.0</v>
-      </c>
-      <c r="E3" s="41"/>
-      <c r="L3" s="42"/>
-    </row>
-    <row r="4" ht="19.5" customHeight="1">
-      <c r="A4" s="39"/>
-      <c r="B4" s="11" t="s">
+      <c r="C3" s="53"/>
+      <c r="D3" s="32">
+        <v>2</v>
+      </c>
+      <c r="E3" s="60"/>
+      <c r="F3" s="53"/>
+      <c r="G3" s="53"/>
+      <c r="H3" s="53"/>
+      <c r="I3" s="53"/>
+      <c r="J3" s="53"/>
+      <c r="K3" s="53"/>
+      <c r="L3" s="68"/>
+    </row>
+    <row r="4" spans="1:12" ht="19.5" customHeight="1">
+      <c r="A4" s="70"/>
+      <c r="B4" s="52" t="s">
         <v>44</v>
       </c>
-      <c r="D4" s="40">
-        <v>2.0</v>
-      </c>
-      <c r="E4" s="41"/>
-      <c r="L4" s="42"/>
-    </row>
-    <row r="5" ht="18.75" customHeight="1">
-      <c r="A5" s="43"/>
-      <c r="B5" s="44" t="s">
+      <c r="C4" s="53"/>
+      <c r="D4" s="32">
+        <v>2</v>
+      </c>
+      <c r="E4" s="60"/>
+      <c r="F4" s="53"/>
+      <c r="G4" s="53"/>
+      <c r="H4" s="53"/>
+      <c r="I4" s="53"/>
+      <c r="J4" s="53"/>
+      <c r="K4" s="53"/>
+      <c r="L4" s="68"/>
+    </row>
+    <row r="5" spans="1:12" ht="18.75" customHeight="1">
+      <c r="A5" s="71"/>
+      <c r="B5" s="54" t="s">
         <v>45</v>
       </c>
-      <c r="C5" s="19"/>
-      <c r="D5" s="45">
-        <v>4.0</v>
-      </c>
-      <c r="E5" s="46"/>
-      <c r="L5" s="42"/>
-    </row>
-    <row r="6" ht="30.75" customHeight="1">
-      <c r="A6" s="31" t="s">
+      <c r="C5" s="55"/>
+      <c r="D5" s="33">
+        <v>4</v>
+      </c>
+      <c r="E5" s="61"/>
+      <c r="F5" s="53"/>
+      <c r="G5" s="53"/>
+      <c r="H5" s="53"/>
+      <c r="I5" s="53"/>
+      <c r="J5" s="53"/>
+      <c r="K5" s="53"/>
+      <c r="L5" s="68"/>
+    </row>
+    <row r="6" spans="1:12" ht="30.75" customHeight="1">
+      <c r="A6" s="69" t="s">
         <v>46</v>
       </c>
-      <c r="B6" s="32" t="s">
+      <c r="B6" s="50" t="s">
         <v>47</v>
       </c>
-      <c r="C6" s="8"/>
-      <c r="D6" s="33">
-        <v>1.0</v>
-      </c>
-      <c r="E6" s="47">
-        <v>2.0</v>
-      </c>
-      <c r="F6" s="35">
-        <v>2.0</v>
-      </c>
-      <c r="G6" s="36">
-        <v>2.0</v>
-      </c>
-      <c r="H6" s="37"/>
-      <c r="I6" s="37"/>
-      <c r="J6" s="37"/>
-      <c r="K6" s="37"/>
-      <c r="L6" s="38"/>
-    </row>
-    <row r="7" ht="29.25" customHeight="1">
-      <c r="A7" s="43"/>
-      <c r="B7" s="44" t="s">
+      <c r="C6" s="51"/>
+      <c r="D6" s="29">
+        <v>1</v>
+      </c>
+      <c r="E6" s="62">
+        <v>2</v>
+      </c>
+      <c r="F6" s="58">
+        <v>2</v>
+      </c>
+      <c r="G6" s="65">
+        <v>2</v>
+      </c>
+      <c r="H6" s="66"/>
+      <c r="I6" s="66"/>
+      <c r="J6" s="66"/>
+      <c r="K6" s="66"/>
+      <c r="L6" s="67"/>
+    </row>
+    <row r="7" spans="1:12" ht="29.25" customHeight="1">
+      <c r="A7" s="71"/>
+      <c r="B7" s="54" t="s">
         <v>48</v>
       </c>
-      <c r="C7" s="19"/>
-      <c r="D7" s="45">
-        <v>1.0</v>
-      </c>
-      <c r="E7" s="46"/>
-      <c r="L7" s="42"/>
-    </row>
-    <row r="8" ht="24.75" customHeight="1">
-      <c r="A8" s="31" t="s">
+      <c r="C7" s="55"/>
+      <c r="D7" s="33">
+        <v>1</v>
+      </c>
+      <c r="E7" s="61"/>
+      <c r="F7" s="53"/>
+      <c r="G7" s="53"/>
+      <c r="H7" s="53"/>
+      <c r="I7" s="53"/>
+      <c r="J7" s="53"/>
+      <c r="K7" s="53"/>
+      <c r="L7" s="68"/>
+    </row>
+    <row r="8" spans="1:12" ht="24.75" customHeight="1">
+      <c r="A8" s="69" t="s">
         <v>49</v>
       </c>
-      <c r="B8" s="32" t="s">
+      <c r="B8" s="50" t="s">
         <v>50</v>
       </c>
-      <c r="C8" s="8"/>
-      <c r="D8" s="33">
-        <v>2.0</v>
-      </c>
-      <c r="E8" s="47">
-        <v>5.0</v>
-      </c>
-      <c r="F8" s="35">
-        <v>3.0</v>
-      </c>
-      <c r="G8" s="36">
-        <v>3.0</v>
-      </c>
-      <c r="H8" s="37"/>
-      <c r="I8" s="37"/>
-      <c r="J8" s="37"/>
-      <c r="K8" s="37"/>
-      <c r="L8" s="38"/>
-    </row>
-    <row r="9" ht="18.75" customHeight="1">
-      <c r="A9" s="43"/>
-      <c r="B9" s="44" t="s">
+      <c r="C8" s="51"/>
+      <c r="D8" s="29">
+        <v>2</v>
+      </c>
+      <c r="E8" s="62">
+        <v>5</v>
+      </c>
+      <c r="F8" s="58">
+        <v>3</v>
+      </c>
+      <c r="G8" s="65">
+        <v>3</v>
+      </c>
+      <c r="H8" s="66"/>
+      <c r="I8" s="66"/>
+      <c r="J8" s="66"/>
+      <c r="K8" s="66"/>
+      <c r="L8" s="67"/>
+    </row>
+    <row r="9" spans="1:12" ht="18.75" customHeight="1">
+      <c r="A9" s="71"/>
+      <c r="B9" s="54" t="s">
         <v>51</v>
       </c>
-      <c r="C9" s="19"/>
-      <c r="D9" s="45">
-        <v>3.0</v>
-      </c>
-      <c r="E9" s="46"/>
-      <c r="L9" s="42"/>
-    </row>
-    <row r="10" ht="20.25" customHeight="1">
-      <c r="A10" s="48" t="s">
+      <c r="C9" s="55"/>
+      <c r="D9" s="33">
+        <v>3</v>
+      </c>
+      <c r="E9" s="61"/>
+      <c r="F9" s="53"/>
+      <c r="G9" s="53"/>
+      <c r="H9" s="53"/>
+      <c r="I9" s="53"/>
+      <c r="J9" s="53"/>
+      <c r="K9" s="53"/>
+      <c r="L9" s="68"/>
+    </row>
+    <row r="10" spans="1:12" ht="20.25" customHeight="1">
+      <c r="A10" s="72" t="s">
         <v>52</v>
       </c>
-      <c r="B10" s="32" t="s">
+      <c r="B10" s="50" t="s">
         <v>53</v>
       </c>
-      <c r="C10" s="8"/>
-      <c r="D10" s="33">
-        <v>4.0</v>
-      </c>
-      <c r="E10" s="47">
-        <v>5.0</v>
-      </c>
-      <c r="F10" s="35">
-        <v>4.0</v>
-      </c>
-      <c r="G10" s="36">
-        <v>4.0</v>
-      </c>
-      <c r="H10" s="37"/>
-      <c r="I10" s="37"/>
-      <c r="J10" s="37"/>
-      <c r="K10" s="37"/>
-      <c r="L10" s="38"/>
-    </row>
-    <row r="11" ht="28.5" customHeight="1">
-      <c r="A11" s="43"/>
-      <c r="B11" s="44" t="s">
+      <c r="C10" s="51"/>
+      <c r="D10" s="29">
+        <v>4</v>
+      </c>
+      <c r="E10" s="62">
+        <v>5</v>
+      </c>
+      <c r="F10" s="58">
+        <v>4</v>
+      </c>
+      <c r="G10" s="65">
+        <v>4</v>
+      </c>
+      <c r="H10" s="66"/>
+      <c r="I10" s="66"/>
+      <c r="J10" s="66"/>
+      <c r="K10" s="66"/>
+      <c r="L10" s="67"/>
+    </row>
+    <row r="11" spans="1:12" ht="28.5" customHeight="1">
+      <c r="A11" s="71"/>
+      <c r="B11" s="54" t="s">
         <v>54</v>
       </c>
-      <c r="C11" s="19"/>
-      <c r="D11" s="45">
-        <v>1.0</v>
-      </c>
-      <c r="E11" s="46"/>
-      <c r="L11" s="42"/>
-    </row>
-    <row r="12" ht="28.5" customHeight="1">
-      <c r="A12" s="49" t="s">
+      <c r="C11" s="55"/>
+      <c r="D11" s="33">
+        <v>1</v>
+      </c>
+      <c r="E11" s="61"/>
+      <c r="F11" s="53"/>
+      <c r="G11" s="53"/>
+      <c r="H11" s="53"/>
+      <c r="I11" s="53"/>
+      <c r="J11" s="53"/>
+      <c r="K11" s="53"/>
+      <c r="L11" s="68"/>
+    </row>
+    <row r="12" spans="1:12" ht="28.5" customHeight="1">
+      <c r="A12" s="73" t="s">
         <v>55</v>
       </c>
-      <c r="B12" s="32" t="s">
+      <c r="B12" s="50" t="s">
         <v>56</v>
       </c>
-      <c r="C12" s="8"/>
-      <c r="D12" s="33">
-        <v>3.0</v>
-      </c>
-      <c r="E12" s="47">
-        <v>6.0</v>
-      </c>
-      <c r="F12" s="35">
-        <v>5.0</v>
-      </c>
-      <c r="G12" s="36">
-        <v>5.0</v>
-      </c>
-      <c r="H12" s="37"/>
-      <c r="I12" s="37"/>
-      <c r="J12" s="37"/>
-      <c r="K12" s="37"/>
-      <c r="L12" s="38"/>
-    </row>
-    <row r="13" ht="31.5" customHeight="1">
-      <c r="A13" s="43"/>
-      <c r="B13" s="44" t="s">
+      <c r="C12" s="51"/>
+      <c r="D12" s="29">
+        <v>3</v>
+      </c>
+      <c r="E12" s="62">
+        <v>6</v>
+      </c>
+      <c r="F12" s="58">
+        <v>5</v>
+      </c>
+      <c r="G12" s="65">
+        <v>5</v>
+      </c>
+      <c r="H12" s="66"/>
+      <c r="I12" s="66"/>
+      <c r="J12" s="66"/>
+      <c r="K12" s="66"/>
+      <c r="L12" s="67"/>
+    </row>
+    <row r="13" spans="1:12" ht="31.5" customHeight="1">
+      <c r="A13" s="71"/>
+      <c r="B13" s="54" t="s">
         <v>57</v>
       </c>
-      <c r="C13" s="19"/>
-      <c r="D13" s="45">
-        <v>3.0</v>
-      </c>
-      <c r="E13" s="46"/>
-      <c r="L13" s="42"/>
-    </row>
-    <row r="14">
-      <c r="A14" s="50" t="s">
+      <c r="C13" s="55"/>
+      <c r="D13" s="33">
+        <v>3</v>
+      </c>
+      <c r="E13" s="61"/>
+      <c r="F13" s="53"/>
+      <c r="G13" s="53"/>
+      <c r="H13" s="53"/>
+      <c r="I13" s="53"/>
+      <c r="J13" s="53"/>
+      <c r="K13" s="53"/>
+      <c r="L13" s="68"/>
+    </row>
+    <row r="14" spans="1:12" ht="57">
+      <c r="A14" s="34" t="s">
         <v>58</v>
       </c>
-      <c r="B14" s="51" t="s">
+      <c r="B14" s="56" t="s">
         <v>59</v>
       </c>
-      <c r="C14" s="27"/>
-      <c r="D14" s="52">
-        <v>5.0</v>
-      </c>
-      <c r="E14" s="53">
-        <v>5.0</v>
-      </c>
-      <c r="F14" s="35">
-        <v>6.0</v>
-      </c>
-      <c r="G14" s="54">
-        <v>6.0</v>
-      </c>
-      <c r="H14" s="37"/>
-      <c r="I14" s="37"/>
-      <c r="J14" s="37"/>
-      <c r="K14" s="37"/>
-      <c r="L14" s="55"/>
-    </row>
-    <row r="15" ht="27.75" customHeight="1">
-      <c r="A15" s="49" t="s">
+      <c r="C14" s="57"/>
+      <c r="D14" s="35">
+        <v>5</v>
+      </c>
+      <c r="E14" s="36">
+        <v>5</v>
+      </c>
+      <c r="F14" s="30">
+        <v>6</v>
+      </c>
+      <c r="G14" s="37">
+        <v>6</v>
+      </c>
+      <c r="H14" s="31"/>
+      <c r="I14" s="31"/>
+      <c r="J14" s="31"/>
+      <c r="K14" s="31"/>
+      <c r="L14" s="38"/>
+    </row>
+    <row r="15" spans="1:12" ht="27.75" customHeight="1">
+      <c r="A15" s="73" t="s">
         <v>60</v>
       </c>
-      <c r="B15" s="32" t="s">
+      <c r="B15" s="50" t="s">
         <v>61</v>
       </c>
-      <c r="C15" s="8"/>
-      <c r="D15" s="33">
-        <v>2.0</v>
-      </c>
-      <c r="E15" s="56">
-        <v>5.0</v>
-      </c>
-      <c r="F15" s="57">
-        <v>7.0</v>
-      </c>
-      <c r="G15" s="36">
-        <v>7.0</v>
-      </c>
-      <c r="H15" s="37"/>
-      <c r="I15" s="37"/>
-      <c r="J15" s="37"/>
-      <c r="K15" s="37"/>
-      <c r="L15" s="38"/>
-    </row>
-    <row r="16" ht="31.5" customHeight="1">
-      <c r="A16" s="43"/>
-      <c r="B16" s="44" t="s">
+      <c r="C15" s="51"/>
+      <c r="D15" s="29">
+        <v>2</v>
+      </c>
+      <c r="E15" s="63">
+        <v>5</v>
+      </c>
+      <c r="F15" s="64">
+        <v>7</v>
+      </c>
+      <c r="G15" s="65">
+        <v>7</v>
+      </c>
+      <c r="H15" s="66"/>
+      <c r="I15" s="66"/>
+      <c r="J15" s="66"/>
+      <c r="K15" s="66"/>
+      <c r="L15" s="67"/>
+    </row>
+    <row r="16" spans="1:12" ht="31.5" customHeight="1">
+      <c r="A16" s="71"/>
+      <c r="B16" s="54" t="s">
         <v>62</v>
       </c>
-      <c r="C16" s="19"/>
-      <c r="D16" s="45">
-        <v>3.0</v>
-      </c>
-      <c r="E16" s="46"/>
-      <c r="L16" s="42"/>
-    </row>
-    <row r="17">
-      <c r="A17" s="50" t="s">
+      <c r="C16" s="55"/>
+      <c r="D16" s="33">
+        <v>3</v>
+      </c>
+      <c r="E16" s="61"/>
+      <c r="F16" s="53"/>
+      <c r="G16" s="53"/>
+      <c r="H16" s="53"/>
+      <c r="I16" s="53"/>
+      <c r="J16" s="53"/>
+      <c r="K16" s="53"/>
+      <c r="L16" s="68"/>
+    </row>
+    <row r="17" spans="1:12" ht="57">
+      <c r="A17" s="34" t="s">
         <v>63</v>
       </c>
-      <c r="B17" s="51" t="s">
+      <c r="B17" s="56" t="s">
         <v>64</v>
       </c>
-      <c r="C17" s="27"/>
-      <c r="D17" s="52">
-        <v>3.0</v>
-      </c>
-      <c r="E17" s="58">
-        <v>3.0</v>
-      </c>
-      <c r="F17" s="57">
-        <v>8.0</v>
-      </c>
-      <c r="G17" s="54">
-        <v>8.0</v>
-      </c>
-      <c r="H17" s="37"/>
-      <c r="I17" s="37"/>
-      <c r="J17" s="37"/>
-      <c r="K17" s="37"/>
-      <c r="L17" s="55"/>
-    </row>
-    <row r="18">
-      <c r="A18" s="50" t="s">
+      <c r="C17" s="57"/>
+      <c r="D17" s="35">
+        <v>3</v>
+      </c>
+      <c r="E17" s="40">
+        <v>3</v>
+      </c>
+      <c r="F17" s="39">
+        <v>8</v>
+      </c>
+      <c r="G17" s="37">
+        <v>8</v>
+      </c>
+      <c r="H17" s="31"/>
+      <c r="I17" s="31"/>
+      <c r="J17" s="31"/>
+      <c r="K17" s="31"/>
+      <c r="L17" s="38"/>
+    </row>
+    <row r="18" spans="1:12" ht="42.75">
+      <c r="A18" s="34" t="s">
         <v>65</v>
       </c>
-      <c r="B18" s="51" t="s">
+      <c r="B18" s="56" t="s">
         <v>66</v>
       </c>
-      <c r="C18" s="27"/>
-      <c r="D18" s="52">
-        <v>3.0</v>
-      </c>
-      <c r="E18" s="53">
-        <v>3.0</v>
-      </c>
-      <c r="F18" s="59">
-        <v>9.0</v>
-      </c>
-      <c r="G18" s="60">
-        <v>9.0</v>
-      </c>
-      <c r="H18" s="61"/>
-      <c r="I18" s="61"/>
-      <c r="J18" s="61"/>
-      <c r="K18" s="61"/>
-      <c r="L18" s="62"/>
-    </row>
-    <row r="19">
-      <c r="E19" s="63"/>
-      <c r="F19" s="64"/>
-    </row>
-    <row r="20">
-      <c r="E20" s="65"/>
-      <c r="F20" s="66"/>
-    </row>
-    <row r="21">
-      <c r="E21" s="63"/>
-      <c r="F21" s="64"/>
-    </row>
-    <row r="22">
-      <c r="E22" s="65"/>
-      <c r="F22" s="66"/>
-    </row>
-    <row r="23">
-      <c r="E23" s="63"/>
-      <c r="F23" s="67"/>
-    </row>
-    <row r="24">
-      <c r="E24" s="65"/>
-      <c r="F24" s="66"/>
-    </row>
-    <row r="25">
-      <c r="E25" s="63"/>
-      <c r="F25" s="64"/>
-    </row>
-    <row r="26">
-      <c r="E26" s="65"/>
-    </row>
-    <row r="27">
-      <c r="E27" s="63"/>
-    </row>
-    <row r="28">
-      <c r="E28" s="65"/>
-    </row>
-    <row r="29">
-      <c r="E29" s="63"/>
-    </row>
-    <row r="30">
-      <c r="E30" s="65"/>
-    </row>
-    <row r="31">
-      <c r="E31" s="63"/>
-    </row>
-    <row r="32">
-      <c r="E32" s="65"/>
-    </row>
-    <row r="33">
-      <c r="E33" s="63"/>
-    </row>
-    <row r="34">
-      <c r="E34" s="65"/>
-    </row>
-    <row r="35">
-      <c r="E35" s="63"/>
-    </row>
-    <row r="36">
-      <c r="E36" s="65"/>
-    </row>
-    <row r="37">
-      <c r="E37" s="63"/>
-    </row>
-    <row r="38">
-      <c r="E38" s="65"/>
-    </row>
-    <row r="39">
-      <c r="E39" s="63"/>
-    </row>
-    <row r="40">
-      <c r="E40" s="65"/>
-    </row>
-    <row r="41">
-      <c r="E41" s="63"/>
-    </row>
-    <row r="42">
-      <c r="E42" s="65"/>
-    </row>
-    <row r="43">
-      <c r="E43" s="63"/>
-    </row>
-    <row r="44">
-      <c r="E44" s="65"/>
-    </row>
-    <row r="45">
-      <c r="E45" s="63"/>
-    </row>
-    <row r="46">
-      <c r="E46" s="65"/>
-    </row>
-    <row r="47">
-      <c r="E47" s="63"/>
-    </row>
-    <row r="48">
-      <c r="E48" s="65"/>
-    </row>
-    <row r="49">
-      <c r="E49" s="63"/>
-    </row>
-    <row r="50">
-      <c r="E50" s="65"/>
-    </row>
-    <row r="51">
-      <c r="E51" s="63"/>
-    </row>
-    <row r="52">
-      <c r="E52" s="65"/>
-    </row>
-    <row r="53">
-      <c r="E53" s="63"/>
-    </row>
-    <row r="54">
-      <c r="E54" s="65"/>
-    </row>
-    <row r="55">
-      <c r="E55" s="63"/>
-    </row>
-    <row r="56">
-      <c r="E56" s="65"/>
-    </row>
-    <row r="57">
-      <c r="E57" s="63"/>
-    </row>
-    <row r="58">
-      <c r="E58" s="65"/>
-    </row>
-    <row r="59">
-      <c r="E59" s="63"/>
-    </row>
-    <row r="60">
-      <c r="E60" s="65"/>
-    </row>
-    <row r="61">
-      <c r="E61" s="63"/>
-    </row>
-    <row r="62">
-      <c r="E62" s="65"/>
-    </row>
-    <row r="63">
-      <c r="E63" s="63"/>
-    </row>
-    <row r="64">
-      <c r="E64" s="65"/>
-    </row>
-    <row r="65">
-      <c r="E65" s="63"/>
-    </row>
-    <row r="66">
-      <c r="E66" s="65"/>
-    </row>
-    <row r="67">
-      <c r="E67" s="63"/>
-    </row>
-    <row r="68">
-      <c r="E68" s="65"/>
-    </row>
-    <row r="69">
-      <c r="E69" s="63"/>
-    </row>
-    <row r="70">
-      <c r="E70" s="65"/>
-    </row>
-    <row r="71">
-      <c r="E71" s="63"/>
-    </row>
-    <row r="72">
-      <c r="E72" s="65"/>
-    </row>
-    <row r="73">
-      <c r="E73" s="63"/>
-    </row>
-    <row r="74">
-      <c r="E74" s="65"/>
-    </row>
-    <row r="75">
-      <c r="E75" s="63"/>
-    </row>
-    <row r="76">
-      <c r="E76" s="65"/>
-    </row>
-    <row r="77">
-      <c r="E77" s="63"/>
-    </row>
-    <row r="78">
-      <c r="E78" s="65"/>
-    </row>
-    <row r="79">
-      <c r="E79" s="63"/>
+      <c r="C18" s="57"/>
+      <c r="D18" s="35">
+        <v>3</v>
+      </c>
+      <c r="E18" s="36">
+        <v>3</v>
+      </c>
+      <c r="F18" s="41">
+        <v>9</v>
+      </c>
+      <c r="G18" s="42">
+        <v>9</v>
+      </c>
+      <c r="H18" s="43"/>
+      <c r="I18" s="43"/>
+      <c r="J18" s="43"/>
+      <c r="K18" s="43"/>
+      <c r="L18" s="44"/>
+    </row>
+    <row r="19" spans="1:12" ht="14.25">
+      <c r="E19" s="45"/>
+      <c r="F19" s="46"/>
+    </row>
+    <row r="20" spans="1:12" ht="14.25">
+      <c r="E20" s="47"/>
+      <c r="F20" s="48"/>
+    </row>
+    <row r="21" spans="1:12" ht="14.25">
+      <c r="E21" s="45"/>
+      <c r="F21" s="46"/>
+    </row>
+    <row r="22" spans="1:12" ht="14.25">
+      <c r="E22" s="47"/>
+      <c r="F22" s="48"/>
+    </row>
+    <row r="23" spans="1:12" ht="14.25">
+      <c r="E23" s="45"/>
+      <c r="F23" s="49"/>
+    </row>
+    <row r="24" spans="1:12" ht="14.25">
+      <c r="E24" s="47"/>
+      <c r="F24" s="48"/>
+    </row>
+    <row r="25" spans="1:12" ht="14.25">
+      <c r="E25" s="45"/>
+      <c r="F25" s="46"/>
+    </row>
+    <row r="26" spans="1:12" ht="14.25">
+      <c r="E26" s="47"/>
+    </row>
+    <row r="27" spans="1:12" ht="14.25">
+      <c r="E27" s="45"/>
+    </row>
+    <row r="28" spans="1:12" ht="14.25">
+      <c r="E28" s="47"/>
+    </row>
+    <row r="29" spans="1:12" ht="14.25">
+      <c r="E29" s="45"/>
+    </row>
+    <row r="30" spans="1:12" ht="14.25">
+      <c r="E30" s="47"/>
+    </row>
+    <row r="31" spans="1:12" ht="14.25">
+      <c r="E31" s="45"/>
+    </row>
+    <row r="32" spans="1:12" ht="14.25">
+      <c r="E32" s="47"/>
+    </row>
+    <row r="33" spans="5:5" ht="14.25">
+      <c r="E33" s="45"/>
+    </row>
+    <row r="34" spans="5:5" ht="14.25">
+      <c r="E34" s="47"/>
+    </row>
+    <row r="35" spans="5:5" ht="14.25">
+      <c r="E35" s="45"/>
+    </row>
+    <row r="36" spans="5:5" ht="14.25">
+      <c r="E36" s="47"/>
+    </row>
+    <row r="37" spans="5:5" ht="14.25">
+      <c r="E37" s="45"/>
+    </row>
+    <row r="38" spans="5:5" ht="14.25">
+      <c r="E38" s="47"/>
+    </row>
+    <row r="39" spans="5:5" ht="14.25">
+      <c r="E39" s="45"/>
+    </row>
+    <row r="40" spans="5:5" ht="14.25">
+      <c r="E40" s="47"/>
+    </row>
+    <row r="41" spans="5:5" ht="14.25">
+      <c r="E41" s="45"/>
+    </row>
+    <row r="42" spans="5:5" ht="14.25">
+      <c r="E42" s="47"/>
+    </row>
+    <row r="43" spans="5:5" ht="14.25">
+      <c r="E43" s="45"/>
+    </row>
+    <row r="44" spans="5:5" ht="14.25">
+      <c r="E44" s="47"/>
+    </row>
+    <row r="45" spans="5:5" ht="14.25">
+      <c r="E45" s="45"/>
+    </row>
+    <row r="46" spans="5:5" ht="14.25">
+      <c r="E46" s="47"/>
+    </row>
+    <row r="47" spans="5:5" ht="14.25">
+      <c r="E47" s="45"/>
+    </row>
+    <row r="48" spans="5:5" ht="14.25">
+      <c r="E48" s="47"/>
+    </row>
+    <row r="49" spans="5:5" ht="14.25">
+      <c r="E49" s="45"/>
+    </row>
+    <row r="50" spans="5:5" ht="14.25">
+      <c r="E50" s="47"/>
+    </row>
+    <row r="51" spans="5:5" ht="14.25">
+      <c r="E51" s="45"/>
+    </row>
+    <row r="52" spans="5:5" ht="14.25">
+      <c r="E52" s="47"/>
+    </row>
+    <row r="53" spans="5:5" ht="14.25">
+      <c r="E53" s="45"/>
+    </row>
+    <row r="54" spans="5:5" ht="14.25">
+      <c r="E54" s="47"/>
+    </row>
+    <row r="55" spans="5:5" ht="14.25">
+      <c r="E55" s="45"/>
+    </row>
+    <row r="56" spans="5:5" ht="14.25">
+      <c r="E56" s="47"/>
+    </row>
+    <row r="57" spans="5:5" ht="14.25">
+      <c r="E57" s="45"/>
+    </row>
+    <row r="58" spans="5:5" ht="14.25">
+      <c r="E58" s="47"/>
+    </row>
+    <row r="59" spans="5:5" ht="14.25">
+      <c r="E59" s="45"/>
+    </row>
+    <row r="60" spans="5:5" ht="14.25">
+      <c r="E60" s="47"/>
+    </row>
+    <row r="61" spans="5:5" ht="14.25">
+      <c r="E61" s="45"/>
+    </row>
+    <row r="62" spans="5:5" ht="14.25">
+      <c r="E62" s="47"/>
+    </row>
+    <row r="63" spans="5:5" ht="14.25">
+      <c r="E63" s="45"/>
+    </row>
+    <row r="64" spans="5:5" ht="14.25">
+      <c r="E64" s="47"/>
+    </row>
+    <row r="65" spans="5:5" ht="14.25">
+      <c r="E65" s="45"/>
+    </row>
+    <row r="66" spans="5:5" ht="14.25">
+      <c r="E66" s="47"/>
+    </row>
+    <row r="67" spans="5:5" ht="14.25">
+      <c r="E67" s="45"/>
+    </row>
+    <row r="68" spans="5:5" ht="14.25">
+      <c r="E68" s="47"/>
+    </row>
+    <row r="69" spans="5:5" ht="14.25">
+      <c r="E69" s="45"/>
+    </row>
+    <row r="70" spans="5:5" ht="14.25">
+      <c r="E70" s="47"/>
+    </row>
+    <row r="71" spans="5:5" ht="14.25">
+      <c r="E71" s="45"/>
+    </row>
+    <row r="72" spans="5:5" ht="14.25">
+      <c r="E72" s="47"/>
+    </row>
+    <row r="73" spans="5:5" ht="14.25">
+      <c r="E73" s="45"/>
+    </row>
+    <row r="74" spans="5:5" ht="14.25">
+      <c r="E74" s="47"/>
+    </row>
+    <row r="75" spans="5:5" ht="14.25">
+      <c r="E75" s="45"/>
+    </row>
+    <row r="76" spans="5:5" ht="14.25">
+      <c r="E76" s="47"/>
+    </row>
+    <row r="77" spans="5:5" ht="14.25">
+      <c r="E77" s="45"/>
+    </row>
+    <row r="78" spans="5:5" ht="14.25">
+      <c r="E78" s="47"/>
+    </row>
+    <row r="79" spans="5:5" ht="14.25">
+      <c r="E79" s="45"/>
     </row>
   </sheetData>
   <mergeCells count="72">
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="F10:F11"/>
-    <mergeCell ref="F12:F13"/>
-    <mergeCell ref="E2:E5"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="F2:F5"/>
-    <mergeCell ref="F15:F16"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="G15:G16"/>
-    <mergeCell ref="I15:I16"/>
-    <mergeCell ref="J15:J16"/>
-    <mergeCell ref="K15:K16"/>
-    <mergeCell ref="L15:L16"/>
-    <mergeCell ref="H15:H16"/>
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="J6:J7"/>
-    <mergeCell ref="K6:K7"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="I8:I9"/>
-    <mergeCell ref="J8:J9"/>
-    <mergeCell ref="K8:K9"/>
+    <mergeCell ref="L2:L5"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="L6:L7"/>
+    <mergeCell ref="I6:I7"/>
     <mergeCell ref="L8:L9"/>
     <mergeCell ref="H8:H9"/>
     <mergeCell ref="G12:G13"/>
@@ -3189,17 +3397,60 @@
     <mergeCell ref="K10:K11"/>
     <mergeCell ref="L10:L11"/>
     <mergeCell ref="H10:H11"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="J6:J7"/>
+    <mergeCell ref="K6:K7"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="I8:I9"/>
+    <mergeCell ref="J8:J9"/>
+    <mergeCell ref="K8:K9"/>
     <mergeCell ref="H2:H5"/>
     <mergeCell ref="H6:H7"/>
     <mergeCell ref="G2:G5"/>
     <mergeCell ref="I2:I5"/>
     <mergeCell ref="J2:J5"/>
     <mergeCell ref="K2:K5"/>
-    <mergeCell ref="L2:L5"/>
-    <mergeCell ref="G6:G7"/>
-    <mergeCell ref="L6:L7"/>
-    <mergeCell ref="I6:I7"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="G15:G16"/>
+    <mergeCell ref="I15:I16"/>
+    <mergeCell ref="J15:J16"/>
+    <mergeCell ref="K15:K16"/>
+    <mergeCell ref="L15:L16"/>
+    <mergeCell ref="H15:H16"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="F2:F5"/>
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="E2:E5"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
   </mergeCells>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>